<commit_message>
Guardando cambios en gg.xlsx
</commit_message>
<xml_diff>
--- a/ProbabilityAndStatistics/gg.xlsx
+++ b/ProbabilityAndStatistics/gg.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge\Desktop\Sem6ULSA\ULSA-6th-Semester\ProbabilityAndStatistics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge\OneDrive\Escritorio\ULSA-6th-Semester\ProbabilityAndStatistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE9A431-554B-42D2-92DC-77B84848658E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFB47E1-2015-48E3-B2D5-A9B2504333A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -19,8 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$2:$B$2</definedName>
     <definedName name="_xlchart.v1.0" hidden="1">Hoja2!$B$2</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Hoja2!$B$3:$B$62</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Hoja2!$B$2</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Hoja2!$B$3:$B$62</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -91,6 +89,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -107,12 +108,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -165,11 +172,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -177,13 +185,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -194,8 +196,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -2124,7 +2136,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="9110870" y="7080803"/>
+              <a:off x="9110870" y="7078732"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2423,17 +2435,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="U31" sqref="U31"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="7"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2450,11 +2462,11 @@
       <c r="B3" s="1">
         <v>2.1</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -2494,7 +2506,7 @@
         <f>COUNTIF($B$3:$B$62,F5)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="4">
         <f>G5/$G$26</f>
         <v>1.6666666666666666E-2</v>
       </c>
@@ -2520,7 +2532,7 @@
         <f t="shared" ref="G6:G25" si="1">COUNTIF($B$3:$B$62,F6)</f>
         <v>2</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="4">
         <f t="shared" ref="H6:H25" si="2">G6/$G$26</f>
         <v>3.3333333333333333E-2</v>
       </c>
@@ -2546,7 +2558,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="4">
         <f t="shared" si="2"/>
         <v>6.6666666666666666E-2</v>
       </c>
@@ -2572,7 +2584,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="4">
         <f t="shared" si="2"/>
         <v>3.3333333333333333E-2</v>
       </c>
@@ -2598,7 +2610,7 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="4">
         <f t="shared" si="2"/>
         <v>8.3333333333333329E-2</v>
       </c>
@@ -2624,7 +2636,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="4">
         <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
@@ -2650,7 +2662,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="4">
         <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
@@ -2676,7 +2688,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="4">
         <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
@@ -2702,7 +2714,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="4">
         <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
@@ -2728,7 +2740,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="4">
         <f t="shared" si="2"/>
         <v>6.6666666666666666E-2</v>
       </c>
@@ -2754,7 +2766,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="4">
         <f t="shared" si="2"/>
         <v>6.6666666666666666E-2</v>
       </c>
@@ -2780,7 +2792,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="4">
         <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
@@ -2806,7 +2818,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="4">
         <f t="shared" si="2"/>
         <v>3.3333333333333333E-2</v>
       </c>
@@ -2832,7 +2844,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="4">
         <f t="shared" si="2"/>
         <v>6.6666666666666666E-2</v>
       </c>
@@ -2858,7 +2870,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="4">
         <f t="shared" si="2"/>
         <v>3.3333333333333333E-2</v>
       </c>
@@ -2884,7 +2896,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H20" s="4">
         <f t="shared" si="2"/>
         <v>6.6666666666666666E-2</v>
       </c>
@@ -2910,7 +2922,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="4">
         <f t="shared" si="2"/>
         <v>3.3333333333333333E-2</v>
       </c>
@@ -2936,7 +2948,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H22" s="4">
         <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
@@ -2962,7 +2974,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H23" s="4">
         <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
@@ -2988,7 +3000,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="H24" s="6">
+      <c r="H24" s="4">
         <f t="shared" si="2"/>
         <v>3.3333333333333333E-2</v>
       </c>
@@ -3014,7 +3026,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H25" s="4">
         <f t="shared" si="2"/>
         <v>1.6666666666666666E-2</v>
       </c>
@@ -3059,14 +3071,14 @@
       <c r="B26" s="1">
         <v>3.8</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="1">
         <f>SUM(G5:G25)</f>
         <v>60</v>
       </c>
-      <c r="H26" s="7">
+      <c r="H26" s="5">
         <f>SUM(H5:H25)</f>
         <v>1</v>
       </c>
@@ -3107,12 +3119,12 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="M28" s="3" t="s">
+      <c r="M28" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
@@ -3137,7 +3149,7 @@
       <c r="O29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P29" s="1" t="s">
+      <c r="P29" s="9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3165,7 +3177,10 @@
         <f>N30+T25</f>
         <v>2.96</v>
       </c>
-      <c r="P30" s="1"/>
+      <c r="P30" s="10">
+        <f>COUNTIFS(B3:B62,"&gt;=2.1",B3:B62,"&lt;=2.96")</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
@@ -3192,7 +3207,10 @@
         <f>N31+T25</f>
         <v>3.8200000000000003</v>
       </c>
-      <c r="P31" s="1"/>
+      <c r="P31" s="10">
+        <f>COUNTIFS(B3:B63,"&gt;=2.96",B3:B63,"&lt;=3.82")</f>
+        <v>25</v>
+      </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
@@ -3219,7 +3237,10 @@
         <f>N32+T25</f>
         <v>4.6800000000000006</v>
       </c>
-      <c r="P32" s="1"/>
+      <c r="P32" s="10">
+        <f>COUNTIFS(B3:B64,"&gt;=3.82",B3:B64,"&lt;=4.68")</f>
+        <v>25</v>
+      </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
@@ -3246,7 +3267,10 @@
         <f>N33+T25</f>
         <v>5.5400000000000009</v>
       </c>
-      <c r="P33" s="1"/>
+      <c r="P33" s="10">
+        <f>COUNTIFS(B3:B65,"&gt;=4.68",B3:B65,"&lt;=5.53")</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
@@ -3273,7 +3297,10 @@
         <f>N34+T25</f>
         <v>6.4000000000000012</v>
       </c>
-      <c r="P34" s="1"/>
+      <c r="P34" s="10">
+        <f>COUNTIFS(F7:F66,"&gt;=5.54",F7:F66,"&lt;=6.4")</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
@@ -3526,7 +3553,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>25</v>
       </c>

</xml_diff>